<commit_message>
Se actualizaron las tablas de presupuesto en el documento...
</commit_message>
<xml_diff>
--- a/05_Lista_Materiales_Herramientas/Presupuestos/Presupuesto_Estimado_[SPT-TD-2025].xlsx
+++ b/05_Lista_Materiales_Herramientas/Presupuestos/Presupuesto_Estimado_[SPT-TD-2025].xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlbertOS\Instituto_Santa_Cruz\Nivel-600\TMG-600\Sistema_Puesta_a_Tierra_Proyecto_AgXplore[SPAT-2025-001]\05_Lista_Materiales_Herramientas\Presupuestos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A92C80-8184-435E-A5FF-C6476D740002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51272671-F559-4BB0-8C0F-FEDA677032BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{0E4B81B5-5C4D-4BDF-BA2C-1E33444AA47B}"/>
   </bookViews>
@@ -434,13 +434,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="2" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -648,21 +648,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -694,17 +694,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1026,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE74045E-23EA-4F9F-95D5-3A8D5F95D7BE}">
   <dimension ref="A3:N105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J64" sqref="J64"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75:G105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,24 +1040,24 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="56"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="28" t="s">
@@ -1128,14 +1128,14 @@
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="53" t="s">
+      <c r="B11" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="55"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="56"/>
     </row>
     <row r="12" spans="2:8" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B12" s="51" t="s">
@@ -1674,14 +1674,14 @@
     </row>
     <row r="38" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="53" t="s">
+      <c r="B39" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="54"/>
-      <c r="D39" s="54"/>
-      <c r="E39" s="54"/>
-      <c r="F39" s="54"/>
-      <c r="G39" s="55"/>
+      <c r="C39" s="55"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="55"/>
+      <c r="F39" s="55"/>
+      <c r="G39" s="56"/>
     </row>
     <row r="40" spans="2:7" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B40" s="51" t="s">
@@ -1869,7 +1869,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>67</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B50" s="7">
         <v>10</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B51" s="7">
         <v>11</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>6250</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B52" s="7">
         <v>12</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B53" s="7">
         <v>13</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B54" s="7">
         <v>14</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B55" s="7">
         <v>15</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B56" s="7">
         <v>16</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B57" s="7">
         <v>17</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B58" s="7">
         <v>18</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B59" s="7">
         <v>19</v>
       </c>
@@ -2092,7 +2092,7 @@
       <c r="F59" s="19"/>
       <c r="G59" s="19"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B60" s="47" t="s">
         <v>15</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>26342</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B61" s="7" t="s">
         <v>85</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>2634.2000000000003</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B62" s="47" t="s">
         <v>16</v>
       </c>
@@ -2136,11 +2136,6 @@
         <v>32400.66</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J63">
-        <v>3</v>
-      </c>
-    </row>
     <row r="71" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="20"/>
       <c r="C71" s="20"/>
@@ -2152,14 +2147,14 @@
     <row r="73" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="74" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="75" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="53" t="s">
+      <c r="B75" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="C75" s="54"/>
-      <c r="D75" s="54"/>
-      <c r="E75" s="54"/>
-      <c r="F75" s="54"/>
-      <c r="G75" s="55"/>
+      <c r="C75" s="55"/>
+      <c r="D75" s="55"/>
+      <c r="E75" s="55"/>
+      <c r="F75" s="55"/>
+      <c r="G75" s="56"/>
     </row>
     <row r="76" spans="2:7" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B76" s="51" t="s">

</xml_diff>